<commit_message>
Update import excel manage user
</commit_message>
<xml_diff>
--- a/public/Sample User Import.xlsx
+++ b/public/Sample User Import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569D577A-6B81-4E73-B915-8166001A3C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE1AF94E-7DB9-42A9-BC16-4C36EE75833A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2169096-B572-4BD3-BBB8-44D5C5E7C866}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
-  <si>
-    <t>Nomor Anggota</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Pangkat</t>
   </si>
@@ -443,7 +440,7 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,7 +457,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -472,95 +469,83 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="1">
-        <v>12345</v>
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1">
         <v>7788999187</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1">
-        <v>12346</v>
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1">
         <v>7788999188</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1">
-        <v>12347</v>
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1">
         <v>7788999189</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>